<commit_message>
Working excel sheet renamer
</commit_message>
<xml_diff>
--- a/Test Modules/Drawing_list.xlsx
+++ b/Test Modules/Drawing_list.xlsx
@@ -370,7 +370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:B7"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -378,38 +378,38 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="B3" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="B4" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="B5" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="B6" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="B7" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>